<commit_message>
Updated BOM to optimize costs
</commit_message>
<xml_diff>
--- a/PCB/SPARC Capstone Preliminary BOM.xlsx
+++ b/PCB/SPARC Capstone Preliminary BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dr_mo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dr_mo\Desktop\School\4th Year\Winter Term\ECE492\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AA38DC-D309-4BD0-A120-2BCFA65FB974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BD81D9-2160-422B-877C-A2EEE5FDA35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2490" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -265,13 +265,13 @@
     <t>$42.39 From Digikey</t>
   </si>
   <si>
-    <t>JP2-JP3</t>
-  </si>
-  <si>
     <t>2057-PH2-06-UA-ND</t>
   </si>
   <si>
     <t>PH2-06-UA</t>
+  </si>
+  <si>
+    <t>JP2-JP5</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -660,13 +660,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -951,7 +948,7 @@
   <dimension ref="B1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,14 +1018,14 @@
         <v>12</v>
       </c>
       <c r="H3" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I3" s="8">
-        <v>0.73</v>
+        <v>0.745</v>
       </c>
       <c r="J3" s="8">
         <f>I3*H3</f>
-        <v>4.38</v>
+        <v>7.45</v>
       </c>
       <c r="K3" s="9"/>
     </row>
@@ -1042,7 +1039,7 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="34" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="26" t="s">
@@ -1052,14 +1049,14 @@
         <v>16</v>
       </c>
       <c r="H4" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I4" s="2">
-        <v>1.38</v>
+        <v>1.07</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ref="J4:J10" si="0">I4*H4</f>
-        <v>5.52</v>
+        <v>10.700000000000001</v>
       </c>
       <c r="K4" s="5"/>
     </row>
@@ -1083,14 +1080,14 @@
         <v>21</v>
       </c>
       <c r="H5" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I5" s="2">
-        <v>0.14000000000000001</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="K5" s="5"/>
     </row>
@@ -1137,7 +1134,7 @@
       <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="35">
         <v>732511150</v>
       </c>
       <c r="F7" s="26" t="s">
@@ -1227,31 +1224,31 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="37" t="s">
+      <c r="B10" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="37">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
       </c>
       <c r="I10" s="2">
         <v>0.19</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>0.19</v>
+        <v>0.38</v>
       </c>
       <c r="K10" s="24"/>
     </row>
@@ -1275,14 +1272,14 @@
         <v>34</v>
       </c>
       <c r="H11" s="1">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="I11" s="3">
-        <v>0.20100000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="J11" s="2">
         <f>I11*H11</f>
-        <v>12.462000000000002</v>
+        <v>8</v>
       </c>
       <c r="K11" s="5"/>
     </row>
@@ -1306,14 +1303,14 @@
         <v>54</v>
       </c>
       <c r="H12" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I12" s="2">
         <v>0.72</v>
       </c>
       <c r="J12" s="2">
         <f>I12*H12</f>
-        <v>2.16</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="K12" s="24"/>
     </row>
@@ -1339,7 +1336,7 @@
       <c r="H13" s="1">
         <v>2</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="36">
         <v>40.270000000000003</v>
       </c>
       <c r="J13" s="2">
@@ -1375,7 +1372,7 @@
       </c>
       <c r="J15" s="20">
         <f>SUM(J3:J13)</f>
-        <v>119.52200000000001</v>
+        <v>125.22000000000001</v>
       </c>
       <c r="K15" s="12"/>
     </row>

</xml_diff>